<commit_message>
Introduced New Tests For The FrameWork
Added:
InvalidLoginTest
AddNewFirstAddressTest
ProductCheckoutTest
SearchProductTest
</commit_message>
<xml_diff>
--- a/testData/LoginData.xlsx
+++ b/testData/LoginData.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13590" windowHeight="6180"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -378,18 +379,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -397,7 +399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>